<commit_message>
db to local ip, etc
</commit_message>
<xml_diff>
--- a/download/records.xlsx
+++ b/download/records.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -445,28 +445,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>2022-11-8</v>
+        <v>2022-11-16</v>
       </c>
       <c r="C2" t="str">
-        <v>HAMIDI</v>
+        <v>idong</v>
       </c>
       <c r="D2" t="str">
-        <v>426903035712000</v>
+        <v>617547260712000</v>
       </c>
       <c r="E2" t="str">
         <v>Orang Pribadi</v>
       </c>
       <c r="F2" t="str">
-        <v>PEMBANGUNAN, KAB. KATINGAN, HAMPALIT, KATINGAN HILIR, KALIMANTAN TENGAH</v>
+        <v>jahanjang</v>
       </c>
       <c r="G2" t="str">
-        <v>PEMBESARAN IKAN AIR TAWAR DI KOLAM</v>
+        <v>karyawan swasta</v>
       </c>
       <c r="H2" t="str">
-        <v>midiehon@gmail.com</v>
+        <v/>
       </c>
       <c r="I2" t="str">
-        <v>Loket 1 (-)</v>
+        <v>Loket 3 (Wiji)</v>
       </c>
       <c r="J2" t="str">
         <v/>
@@ -475,7 +475,7 @@
         <v>Ereg/NPWP</v>
       </c>
       <c r="L2" t="str">
-        <v>Pendaftaran NPWP</v>
+        <v/>
       </c>
     </row>
     <row r="3">
@@ -483,28 +483,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>2022-11-8</v>
+        <v>2022-11-16</v>
       </c>
       <c r="C3" t="str">
-        <v>Krismonitha</v>
+        <v>yesaya</v>
       </c>
       <c r="D3" t="str">
-        <v>616590022712000</v>
+        <v>617694500712000</v>
       </c>
       <c r="E3" t="str">
         <v>Orang Pribadi</v>
       </c>
       <c r="F3" t="str">
-        <v>JL. Tjilik Riwut</v>
+        <v>jl . tangkuhis no. 30</v>
       </c>
       <c r="G3" t="str">
-        <v>Salon Kecantikan</v>
+        <v>karyawan swasta</v>
       </c>
       <c r="H3" t="str">
-        <v>krismonitha_712@mailnesia.com</v>
+        <v/>
       </c>
       <c r="I3" t="str">
-        <v>Loket 4 (Azriel)</v>
+        <v>Loket 3 (Wiji)</v>
       </c>
       <c r="J3" t="str">
         <v/>
@@ -513,7 +513,7 @@
         <v>Ereg/NPWP</v>
       </c>
       <c r="L3" t="str">
-        <v>Pendaftaran</v>
+        <v/>
       </c>
     </row>
     <row r="4">
@@ -521,37 +521,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>2022-11-8</v>
+        <v>2022-11-16</v>
       </c>
       <c r="C4" t="str">
-        <v>DESA TAMPELAS KECAMATAN KAMIPANG KAB. KATINGAN</v>
+        <v>INDRA GANDI</v>
       </c>
       <c r="D4" t="str">
-        <v>001095454712000</v>
+        <v>087179222712000</v>
       </c>
       <c r="E4" t="str">
-        <v>Bendahara</v>
+        <v>Orang Pribadi</v>
       </c>
       <c r="F4" t="str">
-        <v>KANTOR DESA TAMPELAS RT 002 RW 000, KAB. KATINGAN, TAMPELAS, KAMIPANG, KALIMANTAN TENGAH</v>
+        <v>KARUING 001 001, KAB. KATINGAN, KARUING, KAMIPANG, KALIMANTAN TENGAH</v>
       </c>
       <c r="G4" t="str">
-        <v>BENDAHARA LAINNYA YTDL</v>
+        <v>KLU WP Unknown</v>
       </c>
       <c r="H4" t="str">
-        <v>LISAKAYLA91@GMAIL.COM</v>
+        <v/>
       </c>
       <c r="I4" t="str">
-        <v>Loket 2 (Satrio)</v>
+        <v>Loket 3 (Wiji)</v>
       </c>
       <c r="J4" t="str">
         <v/>
       </c>
       <c r="K4" t="str">
-        <v>E-Billing</v>
+        <v>Ereg/NPWP,SPT Tahunan / SPT Masa</v>
       </c>
       <c r="L4" t="str">
-        <v>Billing atas pengadaan melalui dana desa</v>
+        <v/>
       </c>
     </row>
     <row r="5">
@@ -559,42 +559,422 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
+        <v>2022-11-16</v>
+      </c>
+      <c r="C5" t="str">
+        <v>PUTRI NOR MENTARY</v>
+      </c>
+      <c r="D5" t="str">
+        <v>762306215712000</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Orang Pribadi</v>
+      </c>
+      <c r="F5" t="str">
+        <v>DESA PETAK BAHANDANG RT 001 RW 001, KAB. KATINGAN, PETAK BAHANDANG, TASIK PAYAWAN, KALIMANTAN TENGAH</v>
+      </c>
+      <c r="G5" t="str">
+        <v>PEGAWAI SWASTA</v>
+      </c>
+      <c r="H5" t="str">
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <v>Loket 3 (Wiji)</v>
+      </c>
+      <c r="J5" t="str">
+        <v/>
+      </c>
+      <c r="K5" t="str">
+        <v>Ereg/NPWP,SPT Tahunan / SPT Masa</v>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2022-11-15</v>
+      </c>
+      <c r="C6" t="str">
+        <v>NI KADE ANGGARAINI</v>
+      </c>
+      <c r="D6" t="str">
+        <v>086515517712000</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Orang Pribadi</v>
+      </c>
+      <c r="F6" t="str">
+        <v>JALAN KALI SAMBA NO. 025 RT 002, KAB. KATINGAN, TUMBANG KAMAN, SANAMAN MANTIKEI, KALIMANTAN TENGAH</v>
+      </c>
+      <c r="G6" t="str">
+        <v>KLU WP Unknown</v>
+      </c>
+      <c r="H6" t="str">
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <v>Loket 3 (Wiji)</v>
+      </c>
+      <c r="J6" t="str">
+        <v/>
+      </c>
+      <c r="K6" t="str">
+        <v>Ereg/NPWP</v>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2022-11-15</v>
+      </c>
+      <c r="C7" t="str">
+        <v>KRISTIN</v>
+      </c>
+      <c r="D7" t="str">
+        <v>253991624712000</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Orang Pribadi</v>
+      </c>
+      <c r="F7" t="str">
+        <v>JL. A. YANI RT/RW 007/03, KAB. KATINGAN, SAMBA KAHAYAN, KATINGAN TENGAH, KALIMANTAN TENGAH</v>
+      </c>
+      <c r="G7" t="str">
+        <v>KLU WP Unknown</v>
+      </c>
+      <c r="H7" t="str">
+        <v>krist712@mailnesia.com</v>
+      </c>
+      <c r="I7" t="str">
+        <v>Loket 4 (Azriel)</v>
+      </c>
+      <c r="J7" t="str">
+        <v/>
+      </c>
+      <c r="K7" t="str">
+        <v>Ereg/NPWP</v>
+      </c>
+      <c r="L7" t="str">
+        <v>aktivasi efin / djp online &amp; cetak ulang</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2022-11-15</v>
+      </c>
+      <c r="C8" t="str">
+        <v>HANLI</v>
+      </c>
+      <c r="D8" t="str">
+        <v>617407275712000</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Orang Pribadi</v>
+      </c>
+      <c r="F8" t="str">
+        <v>TUMBANG PANGGO</v>
+      </c>
+      <c r="G8" t="str">
+        <v xml:space="preserve">KEBUN, </v>
+      </c>
+      <c r="H8" t="str">
+        <v>hanli712@yopmail.com</v>
+      </c>
+      <c r="I8" t="str">
+        <v>Loket 4 (Azriel)</v>
+      </c>
+      <c r="J8" t="str">
+        <v>NPWP elektronik dikirim lewat WA. WP akan jemput (jika ada waktu)</v>
+      </c>
+      <c r="K8" t="str">
+        <v>Ereg/NPWP</v>
+      </c>
+      <c r="L8" t="str">
+        <v>Daftar NPWP</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>2022-11-15</v>
+      </c>
+      <c r="C9" t="str">
+        <v>RAHMAD FAUZI</v>
+      </c>
+      <c r="D9" t="str">
+        <v>844602268712000</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Orang Pribadi</v>
+      </c>
+      <c r="F9" t="str">
+        <v>JL. TJILIK RIWUT KM. 14</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Dagang</v>
+      </c>
+      <c r="H9" t="str">
+        <v>rahmad712@mailnesia.com</v>
+      </c>
+      <c r="I9" t="str">
+        <v>Loket 4 (Azriel)</v>
+      </c>
+      <c r="J9" t="str">
+        <v/>
+      </c>
+      <c r="K9" t="str">
+        <v>Ereg/NPWP</v>
+      </c>
+      <c r="L9" t="str">
+        <v>cetak ulang npwp (hilang)</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>2022-11-15</v>
+      </c>
+      <c r="C10" t="str">
+        <v>WANDRIE</v>
+      </c>
+      <c r="D10" t="str">
+        <v>321696098712000</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Orang Pribadi</v>
+      </c>
+      <c r="F10" t="str">
+        <v>DESA TEWANG KARANGAN NO. 01 RT 001 RW 001 KEL. PULAU MALAN KASUNGAN 74453 KEC. PULAU MALAN, KAB. KATINGAN, TEWANG KARANGAN, PULAU MALAN, KALIMANTAN TENGAH</v>
+      </c>
+      <c r="G10" t="str">
+        <v>KLU WP Unknown</v>
+      </c>
+      <c r="H10" t="str">
+        <v>wandrie712@yopmail.com</v>
+      </c>
+      <c r="I10" t="str">
+        <v>Loket 4 (Azriel)</v>
+      </c>
+      <c r="J10" t="str">
+        <v>KK : 6206041111100168</v>
+      </c>
+      <c r="K10" t="str">
+        <v>Ereg/NPWP</v>
+      </c>
+      <c r="L10" t="str">
+        <v>Daftar NPWP</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>2022-11-14</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Wiji Thukul</v>
+      </c>
+      <c r="D11" t="str">
+        <v>666666666712000</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Orang Pribadi</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Jl Kasongan Lama</v>
+      </c>
+      <c r="G11" t="str">
+        <v>Tukang bubur</v>
+      </c>
+      <c r="H11" t="str">
+        <v>bruh@bruhmail.com</v>
+      </c>
+      <c r="I11" t="str">
+        <v>Loket 3 (Wiji)</v>
+      </c>
+      <c r="J11" t="str">
+        <v>wp diminta untuk pulang ke rahmatulloh</v>
+      </c>
+      <c r="K11" t="str">
+        <v>E-Billing,SPT Tahunan / SPT Masa</v>
+      </c>
+      <c r="L11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
         <v>2022-11-8</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C12" t="str">
+        <v>HAMIDI</v>
+      </c>
+      <c r="D12" t="str">
+        <v>426903035712000</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Orang Pribadi</v>
+      </c>
+      <c r="F12" t="str">
+        <v>PEMBANGUNAN, KAB. KATINGAN, HAMPALIT, KATINGAN HILIR, KALIMANTAN TENGAH</v>
+      </c>
+      <c r="G12" t="str">
+        <v>PEMBESARAN IKAN AIR TAWAR DI KOLAM</v>
+      </c>
+      <c r="H12" t="str">
+        <v>midiehon@gmail.com</v>
+      </c>
+      <c r="I12" t="str">
+        <v>Loket 1 (-)</v>
+      </c>
+      <c r="J12" t="str">
+        <v/>
+      </c>
+      <c r="K12" t="str">
+        <v>Ereg/NPWP</v>
+      </c>
+      <c r="L12" t="str">
+        <v>Pendaftaran NPWP</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <v>2022-11-8</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Krismonitha</v>
+      </c>
+      <c r="D13" t="str">
+        <v>616590022712000</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Orang Pribadi</v>
+      </c>
+      <c r="F13" t="str">
+        <v>JL. Tjilik Riwut</v>
+      </c>
+      <c r="G13" t="str">
+        <v>Salon Kecantikan</v>
+      </c>
+      <c r="H13" t="str">
+        <v>krismonitha_712@mailnesia.com</v>
+      </c>
+      <c r="I13" t="str">
+        <v>Loket 4 (Azriel)</v>
+      </c>
+      <c r="J13" t="str">
+        <v/>
+      </c>
+      <c r="K13" t="str">
+        <v>Ereg/NPWP</v>
+      </c>
+      <c r="L13" t="str">
+        <v>Pendaftaran</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <v>2022-11-8</v>
+      </c>
+      <c r="C14" t="str">
+        <v>DESA TAMPELAS KECAMATAN KAMIPANG KAB. KATINGAN</v>
+      </c>
+      <c r="D14" t="str">
+        <v>001095454712000</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Bendahara</v>
+      </c>
+      <c r="F14" t="str">
+        <v>KANTOR DESA TAMPELAS RT 002 RW 000, KAB. KATINGAN, TAMPELAS, KAMIPANG, KALIMANTAN TENGAH</v>
+      </c>
+      <c r="G14" t="str">
+        <v>BENDAHARA LAINNYA YTDL</v>
+      </c>
+      <c r="H14" t="str">
+        <v>LISAKAYLA91@GMAIL.COM</v>
+      </c>
+      <c r="I14" t="str">
+        <v>Loket 2 (Satrio)</v>
+      </c>
+      <c r="J14" t="str">
+        <v/>
+      </c>
+      <c r="K14" t="str">
+        <v>E-Billing</v>
+      </c>
+      <c r="L14" t="str">
+        <v>Billing atas pengadaan melalui dana desa</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="str">
+        <v>2022-11-8</v>
+      </c>
+      <c r="C15" t="str">
         <v>HURUNG EKA SAKTI</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D15" t="str">
         <v>021109723712000</v>
       </c>
-      <c r="E5" t="str">
+      <c r="E15" t="str">
         <v>Badan</v>
       </c>
-      <c r="F5" t="str">
+      <c r="F15" t="str">
         <v>JL. KENANGAN NO. 15</v>
       </c>
-      <c r="G5" t="str">
+      <c r="G15" t="str">
         <v>Perkebunan Sawit</v>
       </c>
-      <c r="H5" t="str">
-        <v/>
-      </c>
-      <c r="I5" t="str">
+      <c r="H15" t="str">
+        <v/>
+      </c>
+      <c r="I15" t="str">
         <v>Loket 4 (Azriel)</v>
       </c>
-      <c r="J5" t="str">
+      <c r="J15" t="str">
         <v>Akun djp online (bersama efin) telah disampaikan ke wajib pajak</v>
       </c>
-      <c r="K5" t="str">
-        <v/>
-      </c>
-      <c r="L5" t="str">
+      <c r="K15" t="str">
+        <v/>
+      </c>
+      <c r="L15" t="str">
         <v>Konfirmasi KSWP</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>